<commit_message>
all file update 201601050303
</commit_message>
<xml_diff>
--- a/data/target.xlsx
+++ b/data/target.xlsx
@@ -2111,8 +2111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M47" sqref="M47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2218,35 +2218,33 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>122</v>
+        <v>216</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>123</v>
+        <v>217</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>125</v>
-      </c>
+        <v>212</v>
+      </c>
+      <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>126</v>
+        <v>218</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>120</v>
+        <v>219</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>127</v>
+        <v>220</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>286</v>
+        <v>306</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -2265,35 +2263,35 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>188</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>189</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>190</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>10</v>
+        <v>191</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
-        <v>11</v>
+        <v>192</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>12</v>
+        <v>193</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>13</v>
+        <v>194</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>279</v>
+        <v>306</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -2312,33 +2310,35 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>250</v>
+        <v>33</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>251</v>
+        <v>34</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="F5" s="1"/>
+        <v>35</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>253</v>
+        <v>37</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>254</v>
+        <v>38</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>255</v>
+        <v>39</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>313</v>
+        <v>283</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -2357,33 +2357,33 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>116</v>
+        <v>171</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>117</v>
+        <v>172</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>118</v>
+        <v>173</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>119</v>
+        <v>174</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>120</v>
+        <v>175</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>121</v>
+        <v>176</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
@@ -2402,35 +2402,33 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>323</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>33</v>
+        <v>88</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>34</v>
+        <v>89</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>36</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>39</v>
+        <v>93</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -2449,33 +2447,33 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>323</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>88</v>
+        <v>21</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>89</v>
+        <v>22</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>90</v>
+        <v>23</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>91</v>
+        <v>24</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>92</v>
+        <v>25</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>93</v>
+        <v>26</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
@@ -2494,33 +2492,35 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>205</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>22</v>
+        <v>206</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>24</v>
+        <v>207</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>25</v>
+        <v>208</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>26</v>
+        <v>209</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>281</v>
+        <v>309</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
@@ -2542,29 +2542,27 @@
         <v>316</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>205</v>
+        <v>226</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>206</v>
+        <v>227</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>84</v>
-      </c>
+        <v>228</v>
+      </c>
+      <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>207</v>
+        <v>229</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>208</v>
+        <v>230</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>209</v>
+        <v>231</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>309</v>
@@ -2589,30 +2587,32 @@
         <v>316</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>226</v>
+        <v>122</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>227</v>
+        <v>123</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="F11" s="1"/>
+        <v>124</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>229</v>
+        <v>126</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>230</v>
+        <v>120</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>231</v>
+        <v>127</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>309</v>
+        <v>286</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
@@ -2678,31 +2678,33 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>239</v>
+        <v>210</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>240</v>
+        <v>211</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>241</v>
+        <v>212</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="I13" s="1"/>
+        <v>213</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="J13" s="1" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>287</v>
+        <v>297</v>
       </c>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
@@ -2721,35 +2723,35 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>183</v>
+        <v>140</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>184</v>
+        <v>141</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>130</v>
+        <v>65</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>125</v>
+        <v>142</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1" t="s">
-        <v>185</v>
+        <v>143</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>186</v>
+        <v>144</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>187</v>
+        <v>145</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
@@ -2774,27 +2776,27 @@
         <v>323</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
@@ -2813,35 +2815,35 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>323</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>159</v>
+        <v>7</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>160</v>
+        <v>8</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>161</v>
+        <v>9</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>84</v>
+        <v>10</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1" t="s">
-        <v>162</v>
+        <v>11</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>163</v>
+        <v>12</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>164</v>
+        <v>13</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>301</v>
+        <v>279</v>
       </c>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
@@ -2860,33 +2862,31 @@
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>165</v>
+        <v>239</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>166</v>
+        <v>240</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>167</v>
+        <v>241</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>169</v>
-      </c>
+        <v>242</v>
+      </c>
+      <c r="I17" s="1"/>
       <c r="J17" s="1" t="s">
-        <v>170</v>
+        <v>243</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
@@ -2905,35 +2905,35 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>177</v>
+        <v>57</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>178</v>
+        <v>58</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>155</v>
+        <v>59</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>179</v>
+        <v>36</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1" t="s">
-        <v>180</v>
+        <v>60</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>181</v>
+        <v>61</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>182</v>
+        <v>62</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>304</v>
+        <v>287</v>
       </c>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
@@ -2952,33 +2952,35 @@
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>63</v>
+        <v>183</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>64</v>
+        <v>184</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F19" s="1"/>
+        <v>130</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1" t="s">
-        <v>66</v>
+        <v>185</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>67</v>
+        <v>186</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>68</v>
+        <v>187</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>278</v>
+        <v>305</v>
       </c>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
@@ -2997,37 +2999,35 @@
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>316</v>
+        <v>328</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>244</v>
+        <v>159</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>245</v>
+        <v>160</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>246</v>
+        <v>161</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>3</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="G20" s="1"/>
       <c r="H20" s="1" t="s">
-        <v>247</v>
+        <v>162</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>248</v>
+        <v>163</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>249</v>
+        <v>164</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
@@ -3046,35 +3046,33 @@
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>321</v>
+        <v>329</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>323</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>45</v>
+        <v>165</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>46</v>
+        <v>166</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>36</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1" t="s">
-        <v>48</v>
+        <v>168</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>49</v>
+        <v>169</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>50</v>
+        <v>170</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>285</v>
+        <v>302</v>
       </c>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
@@ -3093,33 +3091,33 @@
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>323</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>69</v>
+        <v>27</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>70</v>
+        <v>28</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>71</v>
+        <v>29</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1" t="s">
-        <v>72</v>
+        <v>30</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>73</v>
+        <v>31</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>74</v>
+        <v>32</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
@@ -3138,35 +3136,35 @@
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>232</v>
+        <v>177</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>233</v>
+        <v>178</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>234</v>
+        <v>155</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>235</v>
+        <v>179</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1" t="s">
-        <v>236</v>
+        <v>180</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>237</v>
+        <v>181</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>238</v>
+        <v>182</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
@@ -3185,35 +3183,33 @@
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>323</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>95</v>
+        <v>64</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>96</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1" t="s">
-        <v>97</v>
+        <v>66</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>98</v>
+        <v>67</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>292</v>
+        <v>278</v>
       </c>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
@@ -3232,35 +3228,31 @@
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>81</v>
+        <v>256</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>82</v>
+        <v>257</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>84</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>86</v>
-      </c>
+        <v>258</v>
+      </c>
+      <c r="I25" s="1"/>
       <c r="J25" s="1" t="s">
-        <v>87</v>
+        <v>259</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>290</v>
+        <v>304</v>
       </c>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
@@ -3279,35 +3271,35 @@
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>323</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>146</v>
+        <v>0</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>147</v>
+        <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="G26" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="H26" s="1" t="s">
-        <v>150</v>
+        <v>4</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>151</v>
+        <v>5</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>152</v>
+        <v>6</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>299</v>
+        <v>278</v>
       </c>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
@@ -3326,33 +3318,33 @@
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>200</v>
+        <v>116</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>201</v>
+        <v>117</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>65</v>
+        <v>118</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1" t="s">
-        <v>202</v>
+        <v>119</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>203</v>
+        <v>120</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>204</v>
+        <v>121</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
@@ -3371,33 +3363,31 @@
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>221</v>
+        <v>40</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>222</v>
+        <v>41</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>224</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="I28" s="1"/>
       <c r="J28" s="1" t="s">
-        <v>225</v>
+        <v>44</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>310</v>
+        <v>284</v>
       </c>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
@@ -3416,16 +3406,16 @@
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>153</v>
+        <v>195</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>154</v>
+        <v>196</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>155</v>
@@ -3433,16 +3423,16 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1" t="s">
-        <v>156</v>
+        <v>197</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>157</v>
+        <v>198</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>158</v>
+        <v>199</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
@@ -3461,33 +3451,33 @@
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>210</v>
+        <v>250</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>211</v>
+        <v>251</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>212</v>
+        <v>252</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1" t="s">
-        <v>213</v>
+        <v>253</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>214</v>
+        <v>254</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>215</v>
+        <v>255</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>297</v>
+        <v>313</v>
       </c>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
@@ -3506,35 +3496,37 @@
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>140</v>
+        <v>244</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>141</v>
+        <v>245</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>65</v>
+        <v>246</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="G31" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="H31" s="1" t="s">
-        <v>143</v>
+        <v>247</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>144</v>
+        <v>248</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>145</v>
+        <v>249</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>297</v>
+        <v>312</v>
       </c>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
@@ -3553,33 +3545,35 @@
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>323</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>51</v>
+        <v>100</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>52</v>
+        <v>101</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F32" s="1"/>
+        <v>59</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1" t="s">
-        <v>54</v>
+        <v>103</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>55</v>
+        <v>104</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>56</v>
+        <v>105</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
@@ -3598,33 +3592,35 @@
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>323</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>113</v>
+        <v>46</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="I33" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="J33" s="1" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
@@ -3646,30 +3642,32 @@
         <v>316</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>171</v>
+        <v>260</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>172</v>
+        <v>261</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="F34" s="1"/>
+        <v>262</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>263</v>
+      </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1" t="s">
-        <v>174</v>
+        <v>264</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>175</v>
+        <v>265</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>176</v>
+        <v>266</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>303</v>
+        <v>314</v>
       </c>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
@@ -3688,35 +3686,33 @@
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>323</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>36</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
@@ -3735,35 +3731,35 @@
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>100</v>
+        <v>232</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>101</v>
+        <v>233</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>59</v>
+        <v>234</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>102</v>
+        <v>235</v>
       </c>
       <c r="G36" s="1"/>
       <c r="H36" s="1" t="s">
-        <v>103</v>
+        <v>236</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>104</v>
+        <v>237</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>105</v>
+        <v>238</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>293</v>
+        <v>311</v>
       </c>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
@@ -3785,28 +3781,32 @@
         <v>321</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>256</v>
+        <v>94</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>257</v>
+        <v>95</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F37" s="1"/>
+      <c r="F37" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="G37" s="1"/>
       <c r="H37" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="I37" s="1"/>
+        <v>97</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="J37" s="1" t="s">
-        <v>259</v>
+        <v>99</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>304</v>
+        <v>292</v>
       </c>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
@@ -3825,35 +3825,35 @@
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>323</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1" t="s">
-        <v>3</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G38" s="1"/>
       <c r="H38" s="1" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>5</v>
+        <v>86</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>278</v>
+        <v>290</v>
       </c>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
@@ -3872,31 +3872,33 @@
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>323</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>40</v>
+        <v>106</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>41</v>
+        <v>107</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>42</v>
+        <v>108</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I39" s="1"/>
+        <v>109</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="J39" s="1" t="s">
-        <v>44</v>
+        <v>111</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>284</v>
+        <v>294</v>
       </c>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
@@ -3918,30 +3920,32 @@
         <v>316</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>195</v>
+        <v>146</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>196</v>
+        <v>147</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="F40" s="1"/>
+        <v>148</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>149</v>
+      </c>
       <c r="G40" s="1"/>
       <c r="H40" s="1" t="s">
-        <v>197</v>
+        <v>150</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>198</v>
+        <v>151</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>199</v>
+        <v>152</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
@@ -3960,35 +3964,33 @@
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>260</v>
+        <v>200</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>261</v>
+        <v>201</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>263</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1" t="s">
-        <v>264</v>
+        <v>202</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>265</v>
+        <v>203</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>266</v>
+        <v>204</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
@@ -4007,33 +4009,35 @@
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>216</v>
+        <v>14</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>217</v>
+        <v>15</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="F42" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G42" s="1"/>
       <c r="H42" s="1" t="s">
-        <v>218</v>
+        <v>18</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>219</v>
+        <v>19</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>220</v>
+        <v>20</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>306</v>
+        <v>280</v>
       </c>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
@@ -4052,33 +4056,33 @@
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>323</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F43" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G43" s="1"/>
       <c r="H43" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>110</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="I43" s="1"/>
       <c r="J43" s="1" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
@@ -4097,35 +4101,33 @@
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>316</v>
+        <v>330</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>188</v>
+        <v>221</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>189</v>
+        <v>222</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>191</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1" t="s">
-        <v>192</v>
+        <v>223</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>193</v>
+        <v>224</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>194</v>
+        <v>225</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
@@ -4144,35 +4146,35 @@
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>323</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>14</v>
+        <v>134</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>15</v>
+        <v>135</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>16</v>
+        <v>136</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>17</v>
+        <v>125</v>
       </c>
       <c r="G45" s="1"/>
       <c r="H45" s="1" t="s">
-        <v>18</v>
+        <v>137</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>19</v>
+        <v>138</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>20</v>
+        <v>139</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>280</v>
+        <v>298</v>
       </c>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
@@ -4191,35 +4193,33 @@
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>323</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>134</v>
+        <v>153</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>125</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="F46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1" t="s">
-        <v>137</v>
+        <v>156</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>138</v>
+        <v>157</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>139</v>
+        <v>158</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
@@ -4413,8 +4413,8 @@
       <c r="Y53" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="A2:K46">
-    <sortCondition ref="C2:C46"/>
+  <sortState ref="A2:K47">
+    <sortCondition ref="K47"/>
   </sortState>
   <phoneticPr fontId="18"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>